<commit_message>
added V spot data for 2019 quarters
</commit_message>
<xml_diff>
--- a/excel_data/Sp19_wk1_A.xlsx
+++ b/excel_data/Sp19_wk1_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Documents\UCSD_old_laptop\Fall_2019\ECE 143\Project\ECE143_FinalProject\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC36DDBD-39A3-414F-8278-F40B9E09E15D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489D9BE1-4884-4E25-BB49-FBB49B7445FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{EC7A8FEE-D0F2-4821-A652-BB6E24BCF2B7}"/>
   </bookViews>
@@ -1110,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD78DD4D-DC8F-43CA-8FE3-05604AABC7F0}">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>